<commit_message>
after baseline and additional information
</commit_message>
<xml_diff>
--- a/documentation/PENUBARTHI-RAPUR-FOREST LANDS.xlsx
+++ b/documentation/PENUBARTHI-RAPUR-FOREST LANDS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ravikiranponduri/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ravikiranponduri/Desktop/GeoPulse/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18DD31DD-6052-614A-A851-A8636BC1937A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{995267CD-DDAB-AD46-B77A-2775F285EDFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="forest_land_vertices" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>lp_no</t>
   </si>
@@ -44,63 +44,6 @@
   </si>
   <si>
     <t>PENUBARTHI VILLAGE RAPUR MANDAL FOREST LAND POINTS DETAILS</t>
-  </si>
-  <si>
-    <t>Before Period Start</t>
-  </si>
-  <si>
-    <t>Before Period End</t>
-  </si>
-  <si>
-    <t>After Period Start</t>
-  </si>
-  <si>
-    <t>After Period End</t>
-  </si>
-  <si>
-    <t>Vegetation (NDVI)-After Value</t>
-  </si>
-  <si>
-    <t>Vegetation (NDVI)-Difference</t>
-  </si>
-  <si>
-    <t>Vegetation (NDVI)-Interpretation</t>
-  </si>
-  <si>
-    <t>Vegetation (NDVI)-Significance</t>
-  </si>
-  <si>
-    <t>Vegetation (NDVI)-Before Value</t>
-  </si>
-  <si>
-    <t>Built-up Area (NDBI)-Before Value</t>
-  </si>
-  <si>
-    <t>Built-up Area (NDBI)-After Value</t>
-  </si>
-  <si>
-    <t>Built-up Area (NDBI)-Difference</t>
-  </si>
-  <si>
-    <t>Built-up Area (NDBI)-Interpretation</t>
-  </si>
-  <si>
-    <t>Built-up Area (NDBI)-Significance</t>
-  </si>
-  <si>
-    <t>Water/Moisture (NDWI)-Before Value</t>
-  </si>
-  <si>
-    <t>Water/Moisture (NDWI)-After Value</t>
-  </si>
-  <si>
-    <t>Water/Moisture (NDWI)-Difference</t>
-  </si>
-  <si>
-    <t>Water/Moisture (NDWI)-Interpretation</t>
-  </si>
-  <si>
-    <t>Water/Moisture (NDWI)-Significance</t>
   </si>
 </sst>
 </file>
@@ -443,10 +386,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z347"/>
+  <dimension ref="A1:G347"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:AA2"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -454,10 +397,10 @@
     <col min="1" max="1" width="8.33203125" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
     <col min="3" max="3" width="10.5" customWidth="1"/>
-    <col min="4" max="1020" width="15"/>
+    <col min="4" max="1000" width="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="16" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="16" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
@@ -468,7 +411,7 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -490,65 +433,8 @@
       <c r="G2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J2" t="s">
-        <v>10</v>
-      </c>
-      <c r="K2" t="s">
-        <v>11</v>
-      </c>
-      <c r="L2" t="s">
-        <v>16</v>
-      </c>
-      <c r="M2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N2" t="s">
-        <v>13</v>
-      </c>
-      <c r="O2" t="s">
-        <v>14</v>
-      </c>
-      <c r="P2" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>17</v>
-      </c>
-      <c r="R2" t="s">
-        <v>18</v>
-      </c>
-      <c r="S2" t="s">
-        <v>19</v>
-      </c>
-      <c r="T2" t="s">
-        <v>20</v>
-      </c>
-      <c r="U2" t="s">
-        <v>21</v>
-      </c>
-      <c r="V2" t="s">
-        <v>22</v>
-      </c>
-      <c r="W2" t="s">
-        <v>23</v>
-      </c>
-      <c r="X2" t="s">
-        <v>24</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>25</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.15">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -571,7 +457,7 @@
         <v>79.523022999999995</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -594,7 +480,7 @@
         <v>79.524128000000005</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -617,7 +503,7 @@
         <v>79.525739999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="1">
         <v>2</v>
       </c>
@@ -640,7 +526,7 @@
         <v>79.526398</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7" s="1">
         <v>2</v>
       </c>
@@ -663,7 +549,7 @@
         <v>79.526929999999993</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="1">
         <v>2</v>
       </c>
@@ -686,7 +572,7 @@
         <v>79.527234000000007</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9" s="1">
         <v>2</v>
       </c>
@@ -709,7 +595,7 @@
         <v>79.526679999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A10" s="1">
         <v>2</v>
       </c>
@@ -732,7 +618,7 @@
         <v>79.526509000000004</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A11" s="1">
         <v>2</v>
       </c>
@@ -755,7 +641,7 @@
         <v>79.525499999999994</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A12" s="1">
         <v>2</v>
       </c>
@@ -778,7 +664,7 @@
         <v>79.524490999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A13" s="1">
         <v>2</v>
       </c>
@@ -801,7 +687,7 @@
         <v>79.523590999999996</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A14" s="1">
         <v>2</v>
       </c>
@@ -824,7 +710,7 @@
         <v>79.522750000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15" s="1">
         <v>2</v>
       </c>
@@ -847,7 +733,7 @@
         <v>79.522307999999995</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16" s="1">
         <v>2</v>
       </c>

</xml_diff>